<commit_message>
create the single profile display page
</commit_message>
<xml_diff>
--- a/admin/docs/dummyalumni.xlsx
+++ b/admin/docs/dummyalumni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/erms/admin/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C8315CA-15AA-F245-A45B-678C941EAB7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3096C0-28E3-D946-B984-16A52F60388A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{3913A13A-1FEF-4141-ABCE-B5840BEF3B0C}"/>
   </bookViews>
@@ -2736,9 +2736,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80E2A72-B1A3-DF4C-BD44-D9C2E7173CFF}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">

</xml_diff>